<commit_message>
build: word-export for clients
</commit_message>
<xml_diff>
--- a/_mat_tz/manures_for_import.xlsx
+++ b/_mat_tz/manures_for_import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_my_projects\manure\_mat_tz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D2E229-FB94-41D6-92E9-1944A989357C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0A77F9-5D98-47F5-BE9C-146F821209FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -469,7 +469,9 @@
       <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1">
+        <v>123</v>
+      </c>
       <c r="C2" s="1">
         <v>3</v>
       </c>

</xml_diff>